<commit_message>
try adding links to PDFs
</commit_message>
<xml_diff>
--- a/Skeena Summer Steelhead Update to Aug _8_24.xlsx
+++ b/Skeena Summer Steelhead Update to Aug _8_24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF2A5B4F-F03E-2E44-AAC8-A0FEC9221A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92182260-4CE1-2E40-8D41-BCB7E322D5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,15 +160,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>183444</xdr:colOff>
+      <xdr:colOff>98778</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>14111</xdr:rowOff>
+      <xdr:rowOff>176678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>323857</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>59797</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>453428</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -191,8 +191,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="183444" y="211667"/>
-          <a:ext cx="7591080" cy="4391908"/>
+          <a:off x="98778" y="374234"/>
+          <a:ext cx="6450650" cy="3732099"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -204,15 +204,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>186267</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>183444</xdr:rowOff>
+      <xdr:colOff>101603</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3685</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>322283</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>174555</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438608</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -235,8 +235,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="186267" y="4924777"/>
-          <a:ext cx="7586683" cy="3942222"/>
+          <a:off x="101603" y="4547463"/>
+          <a:ext cx="6433005" cy="3354759"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -248,15 +248,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>169333</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>16350</xdr:rowOff>
+      <xdr:colOff>98778</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>110513</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>606778</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>125982</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>28222</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -279,8 +279,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="169333" y="9301461"/>
-          <a:ext cx="8565445" cy="4258299"/>
+          <a:off x="98778" y="8407846"/>
+          <a:ext cx="6589889" cy="3276154"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A42:AH176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T72" sqref="T72"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>